<commit_message>
Added excel tools for frame decoding
</commit_message>
<xml_diff>
--- a/frame-bits.xlsx
+++ b/frame-bits.xlsx
@@ -97,9 +97,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -108,6 +105,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41:F66"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A27:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,13 +400,13 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="5">
         <v>0</v>
       </c>
       <c r="C1">
         <v>7</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>80</v>
       </c>
     </row>
@@ -414,11 +414,11 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="5"/>
       <c r="C2">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>40</v>
       </c>
     </row>
@@ -426,11 +426,11 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>20</v>
       </c>
     </row>
@@ -438,11 +438,11 @@
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>10</v>
       </c>
     </row>
@@ -450,11 +450,11 @@
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -462,11 +462,11 @@
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -474,11 +474,11 @@
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="5"/>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -486,11 +486,11 @@
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="5"/>
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -498,13 +498,13 @@
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>80</v>
       </c>
     </row>
@@ -512,11 +512,11 @@
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="5"/>
       <c r="C10">
         <v>6</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>40</v>
       </c>
     </row>
@@ -524,11 +524,11 @@
       <c r="A11">
         <v>11</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="5"/>
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>20</v>
       </c>
     </row>
@@ -536,11 +536,11 @@
       <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="5"/>
       <c r="C12">
         <v>4</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>10</v>
       </c>
     </row>
@@ -548,11 +548,11 @@
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="5"/>
       <c r="C13">
         <v>3</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -560,11 +560,11 @@
       <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="5"/>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -572,11 +572,11 @@
       <c r="A15">
         <v>15</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="5"/>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -584,11 +584,11 @@
       <c r="A16">
         <v>16</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="5"/>
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -596,13 +596,13 @@
       <c r="A17">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="5">
         <v>2</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>80</v>
       </c>
     </row>
@@ -610,11 +610,11 @@
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="5"/>
       <c r="C18">
         <v>6</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>40</v>
       </c>
     </row>
@@ -622,11 +622,11 @@
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="5"/>
       <c r="C19">
         <v>5</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>20</v>
       </c>
     </row>
@@ -634,11 +634,11 @@
       <c r="A20">
         <v>20</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="5"/>
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>10</v>
       </c>
     </row>
@@ -646,11 +646,11 @@
       <c r="A21">
         <v>21</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="5"/>
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -658,11 +658,11 @@
       <c r="A22">
         <v>22</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="5"/>
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -670,11 +670,11 @@
       <c r="A23">
         <v>23</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="5"/>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -682,11 +682,11 @@
       <c r="A24">
         <v>24</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="5"/>
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -694,13 +694,13 @@
       <c r="A25">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="5">
         <v>3</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>80</v>
       </c>
     </row>
@@ -708,11 +708,11 @@
       <c r="A26">
         <v>26</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="5"/>
       <c r="C26">
         <v>6</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>40</v>
       </c>
     </row>
@@ -720,11 +720,11 @@
       <c r="A27">
         <v>27</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="5"/>
       <c r="C27">
         <v>5</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>20</v>
       </c>
     </row>
@@ -732,11 +732,11 @@
       <c r="A28">
         <v>28</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="5"/>
       <c r="C28">
         <v>4</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>10</v>
       </c>
     </row>
@@ -744,11 +744,11 @@
       <c r="A29">
         <v>29</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="5"/>
       <c r="C29">
         <v>3</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -756,11 +756,11 @@
       <c r="A30">
         <v>30</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="5"/>
       <c r="C30">
         <v>2</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -768,11 +768,11 @@
       <c r="A31">
         <v>31</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="5"/>
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -780,11 +780,11 @@
       <c r="A32">
         <v>32</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="5"/>
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -792,13 +792,13 @@
       <c r="A33">
         <v>33</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="5">
         <v>4</v>
       </c>
       <c r="C33">
         <v>7</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>80</v>
       </c>
     </row>
@@ -806,11 +806,11 @@
       <c r="A34">
         <v>34</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="5"/>
       <c r="C34">
         <v>6</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>40</v>
       </c>
     </row>
@@ -818,11 +818,11 @@
       <c r="A35">
         <v>35</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="5"/>
       <c r="C35">
         <v>5</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>20</v>
       </c>
     </row>
@@ -830,11 +830,11 @@
       <c r="A36">
         <v>36</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="5"/>
       <c r="C36">
         <v>4</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>10</v>
       </c>
     </row>
@@ -842,11 +842,11 @@
       <c r="A37">
         <v>37</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="5"/>
       <c r="C37">
         <v>3</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -854,11 +854,11 @@
       <c r="A38">
         <v>38</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="5"/>
       <c r="C38">
         <v>2</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -866,11 +866,11 @@
       <c r="A39">
         <v>39</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="5"/>
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -878,11 +878,11 @@
       <c r="A40">
         <v>40</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="5"/>
       <c r="C40">
         <v>0</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -890,16 +890,16 @@
       <c r="A41">
         <v>41</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="5">
         <v>5</v>
       </c>
       <c r="C41">
         <v>7</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>80</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="E41" s="4"/>
       <c r="F41">
         <v>1</v>
       </c>
@@ -908,14 +908,14 @@
       <c r="A42">
         <v>42</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="5"/>
       <c r="C42">
         <v>6</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>40</v>
       </c>
-      <c r="E42" s="5"/>
+      <c r="E42" s="4"/>
       <c r="F42">
         <v>0</v>
       </c>
@@ -924,14 +924,14 @@
       <c r="A43">
         <v>43</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="5"/>
       <c r="C43">
         <v>5</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>20</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="E43" s="4"/>
       <c r="F43">
         <v>7</v>
       </c>
@@ -940,14 +940,14 @@
       <c r="A44">
         <v>44</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="5"/>
       <c r="C44">
         <v>4</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>10</v>
       </c>
-      <c r="E44" s="5"/>
+      <c r="E44" s="4"/>
       <c r="F44">
         <v>6</v>
       </c>
@@ -956,14 +956,14 @@
       <c r="A45">
         <v>45</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="5"/>
       <c r="C45">
         <v>3</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="5"/>
+      <c r="D45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4"/>
       <c r="F45">
         <v>5</v>
       </c>
@@ -972,14 +972,14 @@
       <c r="A46">
         <v>46</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="5"/>
       <c r="C46">
         <v>2</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="5"/>
+      <c r="D46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="4"/>
       <c r="F46">
         <v>4</v>
       </c>
@@ -988,14 +988,14 @@
       <c r="A47">
         <v>47</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="5"/>
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E47" s="5"/>
+      <c r="D47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="4"/>
       <c r="F47">
         <v>3</v>
       </c>
@@ -1004,14 +1004,14 @@
       <c r="A48">
         <v>48</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="5"/>
       <c r="C48">
         <v>0</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="5"/>
+      <c r="D48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="4"/>
       <c r="F48">
         <v>2</v>
       </c>
@@ -1020,16 +1020,16 @@
       <c r="A49">
         <v>49</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="5">
         <v>6</v>
       </c>
       <c r="C49">
         <v>7</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>80</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="E49" s="4"/>
       <c r="F49">
         <v>1</v>
       </c>
@@ -1038,14 +1038,14 @@
       <c r="A50">
         <v>50</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="5"/>
       <c r="C50">
         <v>6</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>40</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="E50" s="4"/>
       <c r="F50">
         <v>0</v>
       </c>
@@ -1054,14 +1054,14 @@
       <c r="A51">
         <v>51</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="5"/>
       <c r="C51">
         <v>5</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <v>20</v>
       </c>
-      <c r="E51" s="5"/>
+      <c r="E51" s="4"/>
       <c r="F51">
         <v>7</v>
       </c>
@@ -1070,14 +1070,14 @@
       <c r="A52">
         <v>52</v>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="5"/>
       <c r="C52">
         <v>4</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>10</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="E52" s="4"/>
       <c r="F52">
         <v>6</v>
       </c>
@@ -1086,14 +1086,14 @@
       <c r="A53">
         <v>53</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="5"/>
       <c r="C53">
         <v>3</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="5"/>
+      <c r="D53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4"/>
       <c r="F53">
         <v>5</v>
       </c>
@@ -1102,14 +1102,14 @@
       <c r="A54">
         <v>54</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="5"/>
       <c r="C54">
         <v>2</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" s="5"/>
+      <c r="D54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="4"/>
       <c r="F54">
         <v>4</v>
       </c>
@@ -1118,14 +1118,14 @@
       <c r="A55">
         <v>55</v>
       </c>
-      <c r="B55" s="1"/>
+      <c r="B55" s="5"/>
       <c r="C55">
         <v>1</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" s="5"/>
+      <c r="D55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="4"/>
       <c r="F55">
         <v>3</v>
       </c>
@@ -1134,14 +1134,14 @@
       <c r="A56">
         <v>56</v>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="5"/>
       <c r="C56">
         <v>0</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E56" s="5"/>
+      <c r="D56" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="4"/>
       <c r="F56">
         <v>2</v>
       </c>
@@ -1150,16 +1150,16 @@
       <c r="A57">
         <v>57</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="5">
         <v>7</v>
       </c>
       <c r="C57">
         <v>7</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="2">
         <v>80</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="4"/>
       <c r="F57">
         <v>1</v>
       </c>
@@ -1168,14 +1168,14 @@
       <c r="A58">
         <v>58</v>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="5"/>
       <c r="C58">
         <v>6</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="2">
         <v>40</v>
       </c>
-      <c r="E58" s="5"/>
+      <c r="E58" s="4"/>
       <c r="F58">
         <v>0</v>
       </c>
@@ -1184,14 +1184,14 @@
       <c r="A59">
         <v>59</v>
       </c>
-      <c r="B59" s="1"/>
+      <c r="B59" s="5"/>
       <c r="C59">
         <v>5</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="2">
         <v>20</v>
       </c>
-      <c r="E59" s="5"/>
+      <c r="E59" s="4"/>
       <c r="F59">
         <v>7</v>
       </c>
@@ -1200,14 +1200,14 @@
       <c r="A60">
         <v>60</v>
       </c>
-      <c r="B60" s="1"/>
+      <c r="B60" s="5"/>
       <c r="C60">
         <v>4</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="2">
         <v>10</v>
       </c>
-      <c r="E60" s="5"/>
+      <c r="E60" s="4"/>
       <c r="F60">
         <v>6</v>
       </c>
@@ -1216,14 +1216,14 @@
       <c r="A61">
         <v>61</v>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="5"/>
       <c r="C61">
         <v>3</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="5"/>
+      <c r="D61" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="4"/>
       <c r="F61">
         <v>5</v>
       </c>
@@ -1232,14 +1232,14 @@
       <c r="A62">
         <v>62</v>
       </c>
-      <c r="B62" s="1"/>
+      <c r="B62" s="5"/>
       <c r="C62">
         <v>2</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E62" s="5"/>
+      <c r="D62" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" s="4"/>
       <c r="F62">
         <v>4</v>
       </c>
@@ -1248,14 +1248,14 @@
       <c r="A63">
         <v>63</v>
       </c>
-      <c r="B63" s="1"/>
+      <c r="B63" s="5"/>
       <c r="C63">
         <v>1</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E63" s="5"/>
+      <c r="D63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="4"/>
       <c r="F63">
         <v>3</v>
       </c>
@@ -1264,14 +1264,14 @@
       <c r="A64">
         <v>64</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="5"/>
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="5"/>
+      <c r="D64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="4"/>
       <c r="F64">
         <v>2</v>
       </c>
@@ -1280,16 +1280,16 @@
       <c r="A65">
         <v>65</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="5">
         <v>8</v>
       </c>
       <c r="C65">
         <v>7</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="2">
         <v>80</v>
       </c>
-      <c r="E65" s="5"/>
+      <c r="E65" s="4"/>
       <c r="F65">
         <v>1</v>
       </c>
@@ -1298,14 +1298,14 @@
       <c r="A66">
         <v>66</v>
       </c>
-      <c r="B66" s="1"/>
+      <c r="B66" s="5"/>
       <c r="C66">
         <v>6</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="2">
         <v>40</v>
       </c>
-      <c r="E66" s="5"/>
+      <c r="E66" s="4"/>
       <c r="F66">
         <v>0</v>
       </c>
@@ -1314,11 +1314,11 @@
       <c r="A67">
         <v>67</v>
       </c>
-      <c r="B67" s="1"/>
+      <c r="B67" s="5"/>
       <c r="C67">
         <v>5</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="2">
         <v>20</v>
       </c>
       <c r="E67" t="s">
@@ -1329,11 +1329,11 @@
       <c r="A68">
         <v>68</v>
       </c>
-      <c r="B68" s="1"/>
+      <c r="B68" s="5"/>
       <c r="C68">
         <v>4</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="2">
         <v>10</v>
       </c>
       <c r="E68" t="s">
@@ -1344,11 +1344,11 @@
       <c r="A69">
         <v>69</v>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69" s="5"/>
       <c r="C69">
         <v>3</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E69" t="s">
@@ -1359,11 +1359,11 @@
       <c r="A70">
         <v>70</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="5"/>
       <c r="C70">
         <v>2</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E70" t="s">
@@ -1374,11 +1374,11 @@
       <c r="A71">
         <v>71</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="5"/>
       <c r="C71">
         <v>1</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E71" t="s">
@@ -1389,11 +1389,11 @@
       <c r="A72">
         <v>72</v>
       </c>
-      <c r="B72" s="1"/>
+      <c r="B72" s="5"/>
       <c r="C72">
         <v>0</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E72" t="s">
@@ -1404,13 +1404,13 @@
       <c r="A73">
         <v>73</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="5">
         <v>9</v>
       </c>
       <c r="C73">
         <v>7</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="2">
         <v>80</v>
       </c>
       <c r="E73" t="s">
@@ -1421,11 +1421,11 @@
       <c r="A74">
         <v>74</v>
       </c>
-      <c r="B74" s="1"/>
+      <c r="B74" s="5"/>
       <c r="C74">
         <v>6</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="2">
         <v>40</v>
       </c>
       <c r="E74" t="s">
@@ -1436,11 +1436,11 @@
       <c r="A75">
         <v>75</v>
       </c>
-      <c r="B75" s="1"/>
+      <c r="B75" s="5"/>
       <c r="C75">
         <v>5</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="2">
         <v>20</v>
       </c>
       <c r="E75" t="s">
@@ -1451,11 +1451,11 @@
       <c r="A76">
         <v>76</v>
       </c>
-      <c r="B76" s="1"/>
+      <c r="B76" s="5"/>
       <c r="C76">
         <v>4</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="2">
         <v>10</v>
       </c>
       <c r="E76" t="s">
@@ -1466,11 +1466,11 @@
       <c r="A77">
         <v>77</v>
       </c>
-      <c r="B77" s="1"/>
+      <c r="B77" s="5"/>
       <c r="C77">
         <v>3</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E77" t="s">
@@ -1481,11 +1481,11 @@
       <c r="A78">
         <v>78</v>
       </c>
-      <c r="B78" s="1"/>
+      <c r="B78" s="5"/>
       <c r="C78">
         <v>2</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E78" t="s">
@@ -1496,11 +1496,11 @@
       <c r="A79">
         <v>79</v>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="5"/>
       <c r="C79">
         <v>1</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E79" t="s">
@@ -1511,11 +1511,11 @@
       <c r="A80">
         <v>80</v>
       </c>
-      <c r="B80" s="1"/>
+      <c r="B80" s="5"/>
       <c r="C80">
         <v>0</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E80" t="s">
@@ -1526,13 +1526,13 @@
       <c r="A81">
         <v>81</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="5">
         <v>10</v>
       </c>
       <c r="C81">
         <v>7</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="2">
         <v>80</v>
       </c>
       <c r="E81" t="s">
@@ -1543,11 +1543,11 @@
       <c r="A82">
         <v>82</v>
       </c>
-      <c r="B82" s="1"/>
+      <c r="B82" s="5"/>
       <c r="C82">
         <v>6</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="2">
         <v>40</v>
       </c>
       <c r="E82" t="s">
@@ -1558,11 +1558,11 @@
       <c r="A83">
         <v>83</v>
       </c>
-      <c r="B83" s="1"/>
+      <c r="B83" s="5"/>
       <c r="C83">
         <v>5</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D83" s="2">
         <v>20</v>
       </c>
       <c r="E83" t="s">
@@ -1573,11 +1573,11 @@
       <c r="A84">
         <v>84</v>
       </c>
-      <c r="B84" s="1"/>
+      <c r="B84" s="5"/>
       <c r="C84">
         <v>4</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="2">
         <v>10</v>
       </c>
       <c r="E84" t="s">
@@ -1588,11 +1588,11 @@
       <c r="A85">
         <v>85</v>
       </c>
-      <c r="B85" s="1"/>
+      <c r="B85" s="5"/>
       <c r="C85">
         <v>3</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E85" t="s">
@@ -1603,11 +1603,11 @@
       <c r="A86">
         <v>86</v>
       </c>
-      <c r="B86" s="1"/>
+      <c r="B86" s="5"/>
       <c r="C86">
         <v>2</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1615,11 +1615,11 @@
       <c r="A87">
         <v>87</v>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="5"/>
       <c r="C87">
         <v>1</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1627,11 +1627,11 @@
       <c r="A88">
         <v>88</v>
       </c>
-      <c r="B88" s="1"/>
+      <c r="B88" s="5"/>
       <c r="C88">
         <v>0</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1639,13 +1639,13 @@
       <c r="A89">
         <v>89</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="5">
         <v>11</v>
       </c>
       <c r="C89">
         <v>7</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D89" s="2">
         <v>80</v>
       </c>
     </row>
@@ -1653,11 +1653,11 @@
       <c r="A90">
         <v>90</v>
       </c>
-      <c r="B90" s="1"/>
+      <c r="B90" s="5"/>
       <c r="C90">
         <v>6</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1665,11 +1665,11 @@
       <c r="A91">
         <v>91</v>
       </c>
-      <c r="B91" s="1"/>
+      <c r="B91" s="5"/>
       <c r="C91">
         <v>5</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D91" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1677,11 +1677,11 @@
       <c r="A92">
         <v>92</v>
       </c>
-      <c r="B92" s="1"/>
+      <c r="B92" s="5"/>
       <c r="C92">
         <v>4</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D92" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1689,11 +1689,11 @@
       <c r="A93">
         <v>93</v>
       </c>
-      <c r="B93" s="1"/>
+      <c r="B93" s="5"/>
       <c r="C93">
         <v>3</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1701,11 +1701,11 @@
       <c r="A94">
         <v>94</v>
       </c>
-      <c r="B94" s="1"/>
+      <c r="B94" s="5"/>
       <c r="C94">
         <v>2</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1713,11 +1713,11 @@
       <c r="A95">
         <v>95</v>
       </c>
-      <c r="B95" s="1"/>
+      <c r="B95" s="5"/>
       <c r="C95">
         <v>1</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1725,11 +1725,11 @@
       <c r="A96">
         <v>96</v>
       </c>
-      <c r="B96" s="1"/>
+      <c r="B96" s="5"/>
       <c r="C96">
         <v>0</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1737,13 +1737,13 @@
       <c r="A97">
         <v>97</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="5">
         <v>12</v>
       </c>
       <c r="C97">
         <v>7</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="2">
         <v>80</v>
       </c>
     </row>
@@ -1751,11 +1751,11 @@
       <c r="A98">
         <v>98</v>
       </c>
-      <c r="B98" s="1"/>
+      <c r="B98" s="5"/>
       <c r="C98">
         <v>6</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D98" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1763,11 +1763,11 @@
       <c r="A99">
         <v>99</v>
       </c>
-      <c r="B99" s="1"/>
+      <c r="B99" s="5"/>
       <c r="C99">
         <v>5</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1775,11 +1775,11 @@
       <c r="A100">
         <v>100</v>
       </c>
-      <c r="B100" s="1"/>
+      <c r="B100" s="5"/>
       <c r="C100">
         <v>4</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D100" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1787,11 +1787,11 @@
       <c r="A101">
         <v>101</v>
       </c>
-      <c r="B101" s="1"/>
+      <c r="B101" s="5"/>
       <c r="C101">
         <v>3</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="D101" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1799,11 +1799,11 @@
       <c r="A102">
         <v>102</v>
       </c>
-      <c r="B102" s="1"/>
+      <c r="B102" s="5"/>
       <c r="C102">
         <v>2</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1811,11 +1811,11 @@
       <c r="A103">
         <v>103</v>
       </c>
-      <c r="B103" s="1"/>
+      <c r="B103" s="5"/>
       <c r="C103">
         <v>1</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1823,11 +1823,11 @@
       <c r="A104">
         <v>104</v>
       </c>
-      <c r="B104" s="1"/>
+      <c r="B104" s="5"/>
       <c r="C104">
         <v>0</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1835,13 +1835,13 @@
       <c r="A105">
         <v>105</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="5">
         <v>13</v>
       </c>
       <c r="C105">
         <v>7</v>
       </c>
-      <c r="D105" s="3">
+      <c r="D105" s="2">
         <v>80</v>
       </c>
     </row>
@@ -1849,11 +1849,11 @@
       <c r="A106">
         <v>106</v>
       </c>
-      <c r="B106" s="1"/>
+      <c r="B106" s="5"/>
       <c r="C106">
         <v>6</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D106" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1861,11 +1861,11 @@
       <c r="A107">
         <v>107</v>
       </c>
-      <c r="B107" s="1"/>
+      <c r="B107" s="5"/>
       <c r="C107">
         <v>5</v>
       </c>
-      <c r="D107" s="3">
+      <c r="D107" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1873,11 +1873,11 @@
       <c r="A108">
         <v>108</v>
       </c>
-      <c r="B108" s="1"/>
+      <c r="B108" s="5"/>
       <c r="C108">
         <v>4</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1885,11 +1885,11 @@
       <c r="A109">
         <v>109</v>
       </c>
-      <c r="B109" s="1"/>
+      <c r="B109" s="5"/>
       <c r="C109">
         <v>3</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1897,11 +1897,11 @@
       <c r="A110">
         <v>110</v>
       </c>
-      <c r="B110" s="1"/>
+      <c r="B110" s="5"/>
       <c r="C110">
         <v>2</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1909,11 +1909,11 @@
       <c r="A111">
         <v>111</v>
       </c>
-      <c r="B111" s="1"/>
+      <c r="B111" s="5"/>
       <c r="C111">
         <v>1</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1921,11 +1921,11 @@
       <c r="A112">
         <v>112</v>
       </c>
-      <c r="B112" s="1"/>
+      <c r="B112" s="5"/>
       <c r="C112">
         <v>0</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1933,13 +1933,13 @@
       <c r="A113">
         <v>113</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="5">
         <v>14</v>
       </c>
       <c r="C113">
         <v>7</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="2">
         <v>80</v>
       </c>
     </row>
@@ -1947,11 +1947,11 @@
       <c r="A114">
         <v>114</v>
       </c>
-      <c r="B114" s="1"/>
+      <c r="B114" s="5"/>
       <c r="C114">
         <v>6</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D114" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1959,14 +1959,14 @@
       <c r="A115">
         <v>115</v>
       </c>
-      <c r="B115" s="1"/>
+      <c r="B115" s="5"/>
       <c r="C115">
         <v>5</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D115" s="2">
         <v>20</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1974,11 +1974,11 @@
       <c r="A116">
         <v>116</v>
       </c>
-      <c r="B116" s="1"/>
+      <c r="B116" s="5"/>
       <c r="C116">
         <v>4</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D116" s="2">
         <v>10</v>
       </c>
       <c r="E116" t="s">
@@ -1989,11 +1989,11 @@
       <c r="A117">
         <v>117</v>
       </c>
-      <c r="B117" s="1"/>
+      <c r="B117" s="5"/>
       <c r="C117">
         <v>3</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E117" t="s">
@@ -2004,11 +2004,11 @@
       <c r="A118">
         <v>118</v>
       </c>
-      <c r="B118" s="1"/>
+      <c r="B118" s="5"/>
       <c r="C118">
         <v>2</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E118" t="s">
@@ -2019,11 +2019,11 @@
       <c r="A119">
         <v>119</v>
       </c>
-      <c r="B119" s="1"/>
+      <c r="B119" s="5"/>
       <c r="C119">
         <v>1</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E119" t="s">
@@ -2034,11 +2034,11 @@
       <c r="A120">
         <v>120</v>
       </c>
-      <c r="B120" s="1"/>
+      <c r="B120" s="5"/>
       <c r="C120">
         <v>0</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E120" t="s">
@@ -2049,13 +2049,13 @@
       <c r="A121">
         <v>121</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121" s="5">
         <v>15</v>
       </c>
       <c r="C121">
         <v>7</v>
       </c>
-      <c r="D121" s="3">
+      <c r="D121" s="2">
         <v>80</v>
       </c>
       <c r="E121" t="s">
@@ -2066,11 +2066,11 @@
       <c r="A122">
         <v>122</v>
       </c>
-      <c r="B122" s="1"/>
+      <c r="B122" s="5"/>
       <c r="C122">
         <v>6</v>
       </c>
-      <c r="D122" s="3">
+      <c r="D122" s="2">
         <v>40</v>
       </c>
       <c r="E122" t="s">
@@ -2081,11 +2081,11 @@
       <c r="A123">
         <v>123</v>
       </c>
-      <c r="B123" s="1"/>
+      <c r="B123" s="5"/>
       <c r="C123">
         <v>5</v>
       </c>
-      <c r="D123" s="3">
+      <c r="D123" s="2">
         <v>20</v>
       </c>
       <c r="E123" t="s">
@@ -2096,14 +2096,14 @@
       <c r="A124">
         <v>124</v>
       </c>
-      <c r="B124" s="1"/>
+      <c r="B124" s="5"/>
       <c r="C124">
         <v>4</v>
       </c>
-      <c r="D124" s="3">
+      <c r="D124" s="2">
         <v>10</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="E124" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2111,11 +2111,11 @@
       <c r="A125">
         <v>125</v>
       </c>
-      <c r="B125" s="1"/>
+      <c r="B125" s="5"/>
       <c r="C125">
         <v>3</v>
       </c>
-      <c r="D125" s="4" t="s">
+      <c r="D125" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E125" t="s">
@@ -2126,11 +2126,11 @@
       <c r="A126">
         <v>126</v>
       </c>
-      <c r="B126" s="1"/>
+      <c r="B126" s="5"/>
       <c r="C126">
         <v>2</v>
       </c>
-      <c r="D126" s="4" t="s">
+      <c r="D126" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E126" t="s">
@@ -2141,11 +2141,11 @@
       <c r="A127">
         <v>127</v>
       </c>
-      <c r="B127" s="1"/>
+      <c r="B127" s="5"/>
       <c r="C127">
         <v>1</v>
       </c>
-      <c r="D127" s="4" t="s">
+      <c r="D127" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E127" t="s">
@@ -2156,11 +2156,11 @@
       <c r="A128">
         <v>128</v>
       </c>
-      <c r="B128" s="1"/>
+      <c r="B128" s="5"/>
       <c r="C128">
         <v>0</v>
       </c>
-      <c r="D128" s="4" t="s">
+      <c r="D128" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E128" t="s">
@@ -2171,13 +2171,13 @@
       <c r="A129">
         <v>129</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129" s="5">
         <v>16</v>
       </c>
       <c r="C129">
         <v>7</v>
       </c>
-      <c r="D129" s="3">
+      <c r="D129" s="2">
         <v>80</v>
       </c>
       <c r="E129" t="s">
@@ -2188,11 +2188,11 @@
       <c r="A130">
         <v>130</v>
       </c>
-      <c r="B130" s="1"/>
+      <c r="B130" s="5"/>
       <c r="C130">
         <v>6</v>
       </c>
-      <c r="D130" s="3">
+      <c r="D130" s="2">
         <v>40</v>
       </c>
       <c r="E130" t="s">
@@ -2203,11 +2203,11 @@
       <c r="A131">
         <v>131</v>
       </c>
-      <c r="B131" s="1"/>
+      <c r="B131" s="5"/>
       <c r="C131">
         <v>5</v>
       </c>
-      <c r="D131" s="3">
+      <c r="D131" s="2">
         <v>20</v>
       </c>
       <c r="E131" t="s">
@@ -2218,11 +2218,11 @@
       <c r="A132">
         <v>132</v>
       </c>
-      <c r="B132" s="1"/>
+      <c r="B132" s="5"/>
       <c r="C132">
         <v>4</v>
       </c>
-      <c r="D132" s="3">
+      <c r="D132" s="2">
         <v>10</v>
       </c>
       <c r="E132" t="s">
@@ -2233,11 +2233,11 @@
       <c r="A133">
         <v>133</v>
       </c>
-      <c r="B133" s="1"/>
+      <c r="B133" s="5"/>
       <c r="C133">
         <v>3</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D133" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2245,11 +2245,11 @@
       <c r="A134">
         <v>134</v>
       </c>
-      <c r="B134" s="1"/>
+      <c r="B134" s="5"/>
       <c r="C134">
         <v>2</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D134" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2257,11 +2257,11 @@
       <c r="A135">
         <v>135</v>
       </c>
-      <c r="B135" s="1"/>
+      <c r="B135" s="5"/>
       <c r="C135">
         <v>1</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D135" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2269,11 +2269,11 @@
       <c r="A136">
         <v>136</v>
       </c>
-      <c r="B136" s="1"/>
+      <c r="B136" s="5"/>
       <c r="C136">
         <v>0</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D136" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2281,13 +2281,13 @@
       <c r="A137">
         <v>137</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="5">
         <v>17</v>
       </c>
       <c r="C137">
         <v>7</v>
       </c>
-      <c r="D137" s="3">
+      <c r="D137" s="2">
         <v>80</v>
       </c>
     </row>
@@ -2295,11 +2295,11 @@
       <c r="A138">
         <v>138</v>
       </c>
-      <c r="B138" s="1"/>
+      <c r="B138" s="5"/>
       <c r="C138">
         <v>6</v>
       </c>
-      <c r="D138" s="3">
+      <c r="D138" s="2">
         <v>40</v>
       </c>
     </row>
@@ -2307,11 +2307,11 @@
       <c r="A139">
         <v>139</v>
       </c>
-      <c r="B139" s="1"/>
+      <c r="B139" s="5"/>
       <c r="C139">
         <v>5</v>
       </c>
-      <c r="D139" s="3">
+      <c r="D139" s="2">
         <v>20</v>
       </c>
     </row>
@@ -2319,11 +2319,11 @@
       <c r="A140">
         <v>140</v>
       </c>
-      <c r="B140" s="1"/>
+      <c r="B140" s="5"/>
       <c r="C140">
         <v>4</v>
       </c>
-      <c r="D140" s="3">
+      <c r="D140" s="2">
         <v>10</v>
       </c>
     </row>
@@ -2331,11 +2331,11 @@
       <c r="A141">
         <v>141</v>
       </c>
-      <c r="B141" s="1"/>
+      <c r="B141" s="5"/>
       <c r="C141">
         <v>3</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D141" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2343,11 +2343,11 @@
       <c r="A142">
         <v>142</v>
       </c>
-      <c r="B142" s="1"/>
+      <c r="B142" s="5"/>
       <c r="C142">
         <v>2</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D142" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2355,11 +2355,11 @@
       <c r="A143">
         <v>143</v>
       </c>
-      <c r="B143" s="1"/>
+      <c r="B143" s="5"/>
       <c r="C143">
         <v>1</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D143" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2367,27 +2367,16 @@
       <c r="A144">
         <v>144</v>
       </c>
-      <c r="B144" s="1"/>
+      <c r="B144" s="5"/>
       <c r="C144">
         <v>0</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D144" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B137:B144"/>
-    <mergeCell ref="B97:B104"/>
-    <mergeCell ref="B105:B112"/>
-    <mergeCell ref="B113:B120"/>
-    <mergeCell ref="B121:B128"/>
-    <mergeCell ref="B129:B136"/>
-    <mergeCell ref="B49:B56"/>
-    <mergeCell ref="B57:B64"/>
-    <mergeCell ref="B65:B72"/>
-    <mergeCell ref="B73:B80"/>
-    <mergeCell ref="B81:B88"/>
     <mergeCell ref="B89:B96"/>
     <mergeCell ref="B1:B8"/>
     <mergeCell ref="B9:B16"/>
@@ -2395,6 +2384,17 @@
     <mergeCell ref="B25:B32"/>
     <mergeCell ref="B33:B40"/>
     <mergeCell ref="B41:B48"/>
+    <mergeCell ref="B49:B56"/>
+    <mergeCell ref="B57:B64"/>
+    <mergeCell ref="B65:B72"/>
+    <mergeCell ref="B73:B80"/>
+    <mergeCell ref="B81:B88"/>
+    <mergeCell ref="B137:B144"/>
+    <mergeCell ref="B97:B104"/>
+    <mergeCell ref="B105:B112"/>
+    <mergeCell ref="B113:B120"/>
+    <mergeCell ref="B121:B128"/>
+    <mergeCell ref="B129:B136"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>